<commit_message>
Updated lumi projections with new O current
</commit_message>
<xml_diff>
--- a/calculations/results_2025_parameters/005_luminosity_estimates/natalia_2025_data/initial_conditions_SSB.xlsx
+++ b/calculations/results_2025_parameters/005_luminosity_estimates/natalia_2025_data/initial_conditions_SSB.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28919"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="205" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2E13517-764C-4971-A9ED-9AF6229302B6}"/>
+  <xr:revisionPtr revIDLastSave="211" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB09AAF5-C63A-48C5-9A74-F49F010B38B8}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
   <si>
     <t>conservative</t>
   </si>
@@ -51,13 +51,13 @@
     <t>O</t>
   </si>
   <si>
-    <t>7.86e-10​</t>
-  </si>
-  <si>
-    <t>2.87E-6​</t>
-  </si>
-  <si>
-    <t>1.62E9​</t>
+    <t>7.89e-10​</t>
+  </si>
+  <si>
+    <t>2.88E-6​</t>
+  </si>
+  <si>
+    <t>1.81E9​</t>
   </si>
   <si>
     <t>Ar</t>
@@ -264,13 +264,10 @@
     <t>25 ns conservative</t>
   </si>
   <si>
-    <t>7.89e-10​</t>
-  </si>
-  <si>
-    <t>2.88E-6​</t>
-  </si>
-  <si>
-    <t>1.61E9​</t>
+    <t>2.89E-6​</t>
+  </si>
+  <si>
+    <t>1.8E9​</t>
   </si>
   <si>
     <t>4.48E8​</t>
@@ -716,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1028,13 +1025,13 @@
         <v>16</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1051,7 +1048,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1062,13 +1059,13 @@
         <v>40</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1079,13 +1076,13 @@
         <v>86</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1096,13 +1093,13 @@
         <v>115</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1113,13 +1110,13 @@
         <v>129</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1130,13 +1127,13 @@
         <v>208</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>